<commit_message>
@tongnd : commit for Vy
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Tai Lieu_Talent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FFA49A-9BCF-4D07-A460-AA1FAE30A86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49599DE-033F-4FE4-AD9D-7B6336EC3DCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>TestDocs</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Tạo source cho sukien.talenttech6.vn</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -245,25 +248,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -546,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,6 +592,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -598,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E300D9F-F479-4B7B-A40A-032123CECC13}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -619,62 +627,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A3" t="s">
@@ -683,13 +691,13 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F3">
@@ -704,10 +712,10 @@
       <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <v>44022</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>44022</v>
       </c>
     </row>
@@ -718,13 +726,13 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F4">
@@ -739,10 +747,10 @@
       <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>44023</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <v>44023</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add schedule for "Luu"
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Talent\TalentTechDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Tai Lieu_Talent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055B8C80-A1D5-48A6-A96D-DC451FB92269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760515F1-9381-4ED8-8118-5BF3A5E38BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="19200" windowHeight="10180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" sheetId="2" r:id="rId2"/>
-    <sheet name="Master" sheetId="3" r:id="rId3"/>
+    <sheet name="Master" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IT!$B$1:$B$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,24 +28,72 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ADMIN</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{6D5F2848-B438-47C8-8C01-CD60CB628B32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit is Date
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{6B1A951B-967B-40AF-B861-0572EA21C272}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% Actual Percent Of This Task.
+Input 100% if you finished</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>TestDocs</t>
   </si>
   <si>
-    <t>Màn hình quản lý giao dịch</t>
-  </si>
-  <si>
-    <t>Đổi text thành file ngôn ngữ</t>
-  </si>
-  <si>
-    <t>Thêm loại giao dịch SCode</t>
-  </si>
-  <si>
-    <t>Add comment cho method</t>
-  </si>
-  <si>
     <t>Phụ trách</t>
   </si>
   <si>
@@ -53,9 +103,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Số giờ công (người/ngày)</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -120,6 +167,27 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>M_LandingPage</t>
+  </si>
+  <si>
+    <t>M_AboutUs</t>
+  </si>
+  <si>
+    <t>Lưu</t>
+  </si>
+  <si>
+    <t>M_Register</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Chưa có trên mobile / tablet version</t>
+  </si>
+  <si>
+    <t>Person/Day</t>
   </si>
 </sst>
 </file>
@@ -127,9 +195,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="168" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +232,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,7 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -245,10 +326,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,18 +336,320 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -545,214 +924,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="2">
+    <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="0">SUM(F3:H3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="14">
+        <v>44111</v>
+      </c>
+      <c r="K3" s="14">
+        <v>44111</v>
+      </c>
+      <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="14">
+        <v>44112</v>
+      </c>
+      <c r="K4" s="14">
+        <v>44112</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>SUM(F5:H5)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J5" s="14">
+        <v>44113</v>
+      </c>
+      <c r="K5" s="11">
+        <v>44116</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="1">SUM(F6:H6)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J6" s="14">
+        <v>44117</v>
+      </c>
+      <c r="K6" s="13">
+        <v>44118</v>
+      </c>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1.5</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="J7" s="14">
+        <v>44118</v>
+      </c>
+      <c r="K7" s="13">
+        <v>44119</v>
+      </c>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E300D9F-F479-4B7B-A40A-032123CECC13}">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="20.149999999999999" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="20.149999999999999" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.149999999999999" customHeight="1">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.5</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" s="5">
-        <v>44022</v>
-      </c>
-      <c r="K3" s="5">
-        <v>44022</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="20.149999999999999" customHeight="1">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="5">
-        <v>44023</v>
-      </c>
-      <c r="K4" s="5">
-        <v>44023</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
+  <autoFilter ref="B1:B8" xr:uid="{C1DDD69E-323B-4CF4-8844-B9890D7D358F}"/>
   <mergeCells count="10">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -760,30 +1209,95 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="L3:L7">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{FC025A10-0BF8-4EB0-BB0D-8DB07DEA8BD7}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{A8805395-E999-4525-B332-FDE9BA72E8E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,E1)))</xm:f>
+            <xm:f>Master!$C$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,E1)))</xm:f>
+            <xm:f>Master!$C$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,E1)))</xm:f>
+            <xm:f>Master!$C$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
+            <xm:f>$D3=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A3:N8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22B7F516-8BAA-4AF0-8479-6AC1EFCDE90D}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{498507A8-FFF7-4853-B27C-9617AA58C59E}">
+          <x14:formula1>
+            <xm:f>Master!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02CAAD53-6806-422A-96A9-575F68CB0F26}">
           <x14:formula1>
             <xm:f>Master!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D4 D3</xm:sqref>
+          <xm:sqref>D3:D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA1390A7-BBEA-4E10-86CB-52B9315BC1AC}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C020BD32-2477-4C5E-A522-B6AF819E784D}">
           <x14:formula1>
-            <xm:f>Master!$C$2:$C$4</xm:f>
+            <xm:f>Master!$D$2:$D$21</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E4</xm:sqref>
+          <xm:sqref>B5:B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BBFF913-49EC-4E46-B51B-8EF975B4D8A2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DC8D81E-F3FE-4360-B3D1-FE031C309CEE}">
           <x14:formula1>
-            <xm:f>Master!$D$2:$D$3</xm:f>
+            <xm:f>Master!$D$2:$D$10</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B4</xm:sqref>
         </x14:dataValidation>
@@ -793,17 +1307,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B633DAF-049A-473A-B3CD-B37468EBBFEB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -811,40 +1325,43 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Login Test Document
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Tai Lieu_Talent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Talent\TalentTechDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760515F1-9381-4ED8-8118-5BF3A5E38BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8555867-3A6B-4863-B936-D31073EC46B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -336,6 +336,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,146 +356,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -513,139 +394,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -928,67 +676,67 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="7"/>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8"/>
+    <row r="2" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="A2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
@@ -1001,15 +749,15 @@
       <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="L2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
-    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
@@ -1038,15 +786,17 @@
         <f t="shared" ref="I3:I4" si="0">SUM(F3:H3)</f>
         <v>0.5</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="11">
         <v>44111</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="11">
         <v>44111</v>
       </c>
-      <c r="L3" s="15"/>
+      <c r="L3" s="12">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1075,16 +825,16 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="11">
         <v>44112</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>44112</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="N4" s="11"/>
+      <c r="L4" s="12"/>
+      <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1111,18 +861,18 @@
         <f>SUM(F5:H5)</f>
         <v>1.5</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="11">
         <v>44113</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="8">
         <v>44116</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="12"/>
       <c r="N5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="6" spans="1:14" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1149,16 +899,16 @@
         <f t="shared" ref="I6:I7" si="1">SUM(F6:H6)</f>
         <v>1.5</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <v>44117</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="10">
         <v>44118</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:14" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
@@ -1183,15 +933,15 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="11">
         <v>44118</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="10">
         <v>44119</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="8" spans="1:14" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
     </row>
@@ -1210,7 +960,7 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L7">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1315,9 +1065,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Bao cao tien do o schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/TalentTechDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Desktop\Talent\TalentTechDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78168B03-1A44-EB4F-B7C3-B33CC4D6B1F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186A8BEC-D956-48B3-8797-2E66995D3766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -444,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -483,6 +483,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,20 +493,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -545,6 +539,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -882,70 +883,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="19.5" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="23.5" customWidth="1"/>
-    <col min="14" max="18" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
+    <col min="14" max="18" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="17"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
+    <row r="2" spans="1:14" ht="14.5">
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
@@ -958,15 +959,15 @@
       <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" ht="15">
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.5">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14" ht="14.5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1121,7 +1122,7 @@
       </c>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -1164,7 +1165,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="20" customHeight="1">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1174,7 +1175,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
@@ -1184,6 +1185,9 @@
       </c>
       <c r="K8" s="9">
         <v>44119</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -1350,64 +1354,64 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="61.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="61.6328125" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>23</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="17"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="13" t="s">
         <v>19</v>
       </c>
@@ -1420,13 +1424,13 @@
       <c r="I2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -1474,7 +1478,7 @@
       <c r="L5" s="10"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1">
+    <row r="6" spans="1:14" ht="15" thickBot="1">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -1483,7 +1487,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -1507,12 +1511,12 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L6">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula xml:space="preserve"> AND(L7&lt;100, K7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1612,7 +1616,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1632,9 +1636,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
add fix bug LD_Home
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\LuuDV\TalentTechDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/TalentTechDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6310B4-A584-4EB5-8352-8F9604F12A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24A2BB3-3C5B-934A-81E4-8BE4CB9FD7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,12 @@
     <sheet name="Master" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IT!$B$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IT!$C$1:$C$7</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -42,7 +36,7 @@
     <author>ADMIN</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{6D5F2848-B438-47C8-8C01-CD60CB628B32}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{6D5F2848-B438-47C8-8C01-CD60CB628B32}">
       <text>
         <r>
           <rPr>
@@ -67,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{6B1A951B-967B-40AF-B861-0572EA21C272}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{6B1A951B-967B-40AF-B861-0572EA21C272}">
       <text>
         <r>
           <rPr>
@@ -157,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>TestDocs</t>
   </si>
@@ -192,12 +186,6 @@
     <t>Tòng</t>
   </si>
   <si>
-    <t>Test Login Page</t>
-  </si>
-  <si>
-    <t>Create Login Test Document</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -237,12 +225,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>M_LandingPage</t>
-  </si>
-  <si>
-    <t>M_AboutUs</t>
-  </si>
-  <si>
     <t>Lưu</t>
   </si>
   <si>
@@ -252,13 +234,7 @@
     <t>Person/Day</t>
   </si>
   <si>
-    <t>User Test: Tìm lỗi (Mobile)</t>
-  </si>
-  <si>
     <t>https://talenttech6.vn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chỉ cần ghi lỗi vào 1 file txt </t>
   </si>
   <si>
     <t>x</t>
@@ -294,13 +270,37 @@
     </r>
   </si>
   <si>
-    <t>M_LandingPage_Test</t>
-  </si>
-  <si>
     <t>sukien.talenttech6.com</t>
   </si>
   <si>
     <t>15/10/2020</t>
+  </si>
+  <si>
+    <t>Mobile, Web (DONE), Tablet (Not Yet)</t>
+  </si>
+  <si>
+    <t>Fix Kadai</t>
+  </si>
+  <si>
+    <t>T6_Login_Test</t>
+  </si>
+  <si>
+    <t>T6_Login_PT</t>
+  </si>
+  <si>
+    <t>T6_User Test (Mobile)</t>
+  </si>
+  <si>
+    <t>LD_Home_Cd</t>
+  </si>
+  <si>
+    <t>LD_AboutUs_Cd</t>
+  </si>
+  <si>
+    <t>LD_Home_Test</t>
+  </si>
+  <si>
+    <t>LD_Home_Bug</t>
   </si>
 </sst>
 </file>
@@ -310,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,13 @@
       <strike/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -503,12 +510,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -548,6 +558,55 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -890,347 +949,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="18" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="19" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:15" ht="20" customHeight="1">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="15">
+      <c r="B2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15">
-      <c r="A2" s="19"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="18"/>
       <c r="N2" s="18"/>
-    </row>
-    <row r="3" spans="1:14" ht="15">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I4" si="0">SUM(F3:H3)</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J4" si="0">SUM(G3:I3)</f>
         <v>0.5</v>
-      </c>
-      <c r="J3" s="9">
-        <v>44111</v>
       </c>
       <c r="K3" s="9">
         <v>44111</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
+        <v>44111</v>
+      </c>
+      <c r="M3" s="10">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J4" s="9">
-        <v>44112</v>
-      </c>
       <c r="K4" s="9">
         <v>44112</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" ht="81" customHeight="1">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5">
+      <c r="L4" s="9">
+        <v>44112</v>
+      </c>
+      <c r="M4" s="10">
+        <v>100</v>
+      </c>
+      <c r="N4" s="21">
+        <v>44112</v>
+      </c>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" ht="81" customHeight="1">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <f>SUM(F5:H5)</f>
+      <c r="J5">
+        <f>SUM(G5:I5)</f>
         <v>1.5</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="9">
         <v>44113</v>
       </c>
-      <c r="K5" s="9">
+      <c r="L5" s="9">
         <v>44117</v>
       </c>
-      <c r="L5" s="10">
+      <c r="M5" s="10">
         <v>100</v>
       </c>
-      <c r="M5" s="14">
+      <c r="N5" s="14">
         <v>44118</v>
       </c>
-      <c r="N5" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6">
+      <c r="O5" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="20" customHeight="1" thickBot="1">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6" si="1">SUM(F6:H6)</f>
+      <c r="J6">
+        <f t="shared" ref="J6" si="1">SUM(G6:I6)</f>
         <v>1.5</v>
-      </c>
-      <c r="J6" s="9">
-        <v>44118</v>
       </c>
       <c r="K6" s="9">
         <v>44118</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
+        <v>44118</v>
+      </c>
+      <c r="M6" s="10">
         <v>100</v>
       </c>
-      <c r="M6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="N6" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16" thickBot="1">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="I7">
-        <f t="shared" ref="I7" si="2">SUM(F7:H7)</f>
+      <c r="J7">
+        <f t="shared" ref="J7" si="2">SUM(G7:I7)</f>
         <v>1</v>
       </c>
-      <c r="J7" s="9">
+      <c r="K7" s="9">
         <v>44113</v>
       </c>
-      <c r="K7" s="9">
+      <c r="L7" s="9">
         <v>44116</v>
       </c>
-      <c r="L7" s="10">
-        <v>40</v>
-      </c>
-      <c r="N7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="M7" s="10">
+        <v>100</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="9">
-        <v>44119</v>
+      <c r="B8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="K8" s="9">
         <v>44119</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M8" s="17">
         <v>0.6</v>
       </c>
+      <c r="N8" s="14"/>
+      <c r="O8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="20" customHeight="1">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="9">
+        <v>44120</v>
+      </c>
+      <c r="L9" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="14"/>
+      <c r="O9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="20" customHeight="1">
+      <c r="N10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" ht="20" customHeight="1">
+      <c r="N11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" ht="20" customHeight="1">
+      <c r="N12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" ht="20" customHeight="1">
+      <c r="N13" s="14"/>
+    </row>
+    <row r="14" spans="1:15" ht="20" customHeight="1">
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" ht="20" customHeight="1">
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:15" ht="20" customHeight="1">
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="14:14" ht="20" customHeight="1">
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="14:14" ht="20" customHeight="1">
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="14:14" ht="20" customHeight="1">
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="14:14" ht="20" customHeight="1">
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="14:14" ht="20" customHeight="1">
+      <c r="N21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:L6">
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
+  <conditionalFormatting sqref="M3:M6">
+    <cfRule type="expression" dxfId="21" priority="14">
+      <formula xml:space="preserve"> AND(M3&lt;100, L3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="13" priority="4">
-      <formula xml:space="preserve"> AND(L7&lt;100, K7 &lt; TODAY())</formula>
+  <conditionalFormatting sqref="M7">
+    <cfRule type="expression" dxfId="20" priority="11">
+      <formula xml:space="preserve"> AND(M7&lt;100, L7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{FC025A10-0BF8-4EB0-BB0D-8DB07DEA8BD7}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{A8805395-E999-4525-B332-FDE9BA72E8E9}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{210509F4-CBFC-4922-9ED9-192EFD2DBDC2}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{FC025A10-0BF8-4EB0-BB0D-8DB07DEA8BD7}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{A8805395-E999-4525-B332-FDE9BA72E8E9}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{210509F4-CBFC-4922-9ED9-192EFD2DBDC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1239,8 +1390,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,E1)))</xm:f>
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F1)))</xm:f>
             <xm:f>Master!$C$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1250,8 +1401,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,E1)))</xm:f>
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F1)))</xm:f>
             <xm:f>Master!$C$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1261,8 +1412,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,E1)))</xm:f>
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F1)))</xm:f>
             <xm:f>Master!$C$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1272,11 +1423,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>F1:F8 F10:F1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
-            <xm:f>$D3=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="12" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
+            <xm:f>$E3=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1285,11 +1436,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A3:N4 A5:J6 L6:M6 L5 A8 E7:E8</xm:sqref>
+          <xm:sqref>B5:K6 M5:M6 B8 C7:C8 B3:O4 F7:F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
-            <xm:f>$D5=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="10" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
+            <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1298,11 +1449,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K5:K7</xm:sqref>
+          <xm:sqref>L5:L7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
-            <xm:f>$D5=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="9" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
+            <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1311,11 +1462,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>M5</xm:sqref>
+          <xm:sqref>N5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{B31F4DC5-7A8C-804B-89A6-941728D02FBD}">
-            <xm:f>$D8=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="8" id="{B31F4DC5-7A8C-804B-89A6-941728D02FBD}">
+            <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1324,7 +1475,95 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D8</xm:sqref>
+          <xm:sqref>E8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{5EDD22EA-270F-064D-9ACE-ACAC46F7D7D3}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F9)))</xm:f>
+            <xm:f>Master!$C$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{30D1F81A-DEC7-E444-96B7-C79FBC52E21B}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F9)))</xm:f>
+            <xm:f>Master!$C$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{B3F98871-AEB5-664B-8DE2-9210588F29DB}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F9)))</xm:f>
+            <xm:f>Master!$C$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{CCCC3B6D-E61F-CE41-9FC8-5896F04EB6CF}">
+            <xm:f>$E9=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{B73FD618-63AE-DF4C-A7CA-7FD2F8AE6608}">
+            <xm:f>$E9=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{5669D208-A0FB-3B42-B58D-7CCD73284DA4}">
+            <xm:f>$E9=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{EF4FC66B-04B7-8842-94D2-380B3463E6E7}">
+            <xm:f>$E6=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N6:N21</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1334,25 +1573,25 @@
           <x14:formula1>
             <xm:f>Master!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E8</xm:sqref>
+          <xm:sqref>F3:F9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02CAAD53-6806-422A-96A9-575F68CB0F26}">
           <x14:formula1>
             <xm:f>Master!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D6 D8</xm:sqref>
+          <xm:sqref>E3:E6 E8:E9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C020BD32-2477-4C5E-A522-B6AF819E784D}">
           <x14:formula1>
             <xm:f>Master!$D$2:$D$21</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B6</xm:sqref>
+          <xm:sqref>C5:C9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DC8D81E-F3FE-4360-B3D1-FE031C309CEE}">
           <x14:formula1>
             <xm:f>Master!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B4</xm:sqref>
+          <xm:sqref>C3:C4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1368,18 +1607,18 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.5" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1399,25 +1638,25 @@
         <v>8</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>23</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1427,38 +1666,38 @@
       <c r="D2" s="20"/>
       <c r="E2" s="18"/>
       <c r="F2" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -1466,10 +1705,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -1481,7 +1720,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -1492,7 +1731,7 @@
       <c r="L5" s="10"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1">
+    <row r="6" spans="1:14" ht="16" thickBot="1">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -1501,7 +1740,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+    <row r="7" spans="1:14" ht="16" thickBot="1">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -1630,11 +1869,11 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1650,9 +1889,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1668,10 +1907,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1679,10 +1918,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1690,13 +1929,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add "About Us" Test
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/TalentTechDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24A2BB3-3C5B-934A-81E4-8BE4CB9FD7D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D23368-1DDD-444B-B5D9-69B1342BCFDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>TestDocs</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>LD_Home_Bug</t>
+  </si>
+  <si>
+    <t>LD_AboutUs_Test</t>
+  </si>
+  <si>
+    <t>Mobile, Web, Tablet</t>
   </si>
 </sst>
 </file>
@@ -460,7 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -499,8 +505,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,15 +517,173 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -951,70 +1116,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" customWidth="1"/>
-    <col min="14" max="14" width="23.5" customWidth="1"/>
-    <col min="15" max="19" width="35.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="19" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20" customHeight="1">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="B1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>21</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15">
-      <c r="B2" s="19"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1027,13 +1192,13 @@
       <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
       <c r="M2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="1:15" ht="15">
       <c r="A3">
@@ -1118,7 +1283,7 @@
       <c r="M4" s="10">
         <v>100</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="16">
         <v>44112</v>
       </c>
       <c r="O4" s="6"/>
@@ -1169,7 +1334,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="20" customHeight="1" thickBot="1">
+    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1212,11 +1377,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16" thickBot="1">
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1225,8 +1390,8 @@
       <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>12</v>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>16</v>
@@ -1255,17 +1420,17 @@
       </c>
       <c r="N7" s="14"/>
     </row>
-    <row r="8" spans="1:15" ht="20" customHeight="1">
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1274,31 +1439,34 @@
       <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
       <c r="K8" s="9">
         <v>44119</v>
       </c>
       <c r="L8" s="9">
         <v>44120</v>
       </c>
-      <c r="M8" s="17">
-        <v>0.6</v>
+      <c r="M8" s="10">
+        <v>60</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="20" customHeight="1">
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1307,52 +1475,166 @@
       <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
       <c r="K9" s="9">
         <v>44120</v>
       </c>
       <c r="L9" s="9">
         <v>44120</v>
       </c>
-      <c r="M9" s="17"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="14"/>
       <c r="O9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="20" customHeight="1">
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9">
+        <v>44120</v>
+      </c>
+      <c r="L10" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M10" s="10"/>
       <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" ht="20" customHeight="1">
+      <c r="O10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M11" s="10"/>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:15" ht="20" customHeight="1">
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M12" s="10"/>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:15" ht="20" customHeight="1">
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M13" s="10"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:15" ht="20" customHeight="1">
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M14" s="10"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="20" customHeight="1">
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M15" s="10"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:15" ht="20" customHeight="1">
+    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M16" s="10"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="14:14" ht="20" customHeight="1">
+    <row r="17" spans="4:14" ht="20.100000000000001" customHeight="1">
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M17" s="10"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="14:14" ht="20" customHeight="1">
+    <row r="18" spans="4:14" ht="20.100000000000001" customHeight="1">
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M18" s="10"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="14:14" ht="20" customHeight="1">
+    <row r="19" spans="4:14" ht="20.100000000000001" customHeight="1">
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M19" s="10"/>
       <c r="N19" s="14"/>
     </row>
-    <row r="20" spans="14:14" ht="20" customHeight="1">
+    <row r="20" spans="4:14" ht="20.100000000000001" customHeight="1">
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9">
+        <v>44120</v>
+      </c>
+      <c r="M20" s="10"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="14:14" ht="20" customHeight="1">
+    <row r="21" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="N21" s="14"/>
     </row>
   </sheetData>
@@ -1369,13 +1651,18 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" dxfId="21" priority="14">
+    <cfRule type="expression" dxfId="44" priority="37">
       <formula xml:space="preserve"> AND(M3&lt;100, L3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula xml:space="preserve"> AND(M7&lt;100, L7 &lt; TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8:M20">
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula xml:space="preserve"> AND(M8&lt;100, L8 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -1390,7 +1677,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
+          <x14:cfRule type="containsText" priority="38" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F1)))</xm:f>
             <xm:f>Master!$C$4</xm:f>
             <x14:dxf>
@@ -1401,7 +1688,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
+          <x14:cfRule type="containsText" priority="39" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F1)))</xm:f>
             <xm:f>Master!$C$3</xm:f>
             <x14:dxf>
@@ -1412,7 +1699,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
+          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F1)))</xm:f>
             <xm:f>Master!$C$2</xm:f>
             <x14:dxf>
@@ -1423,10 +1710,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F1:F8 F10:F1048576</xm:sqref>
+          <xm:sqref>F1:F6 F21:F1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="12" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
+          <x14:cfRule type="expression" priority="35" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
             <xm:f>$E3=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1436,10 +1723,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B5:K6 M5:M6 B8 C7:C8 B3:O4 F7:F9</xm:sqref>
+          <xm:sqref>B5:K6 M5:M6 B3:O4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="10" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
+          <x14:cfRule type="expression" priority="33" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
             <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1449,10 +1736,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>L5:L7</xm:sqref>
+          <xm:sqref>L5:L6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
+          <x14:cfRule type="expression" priority="32" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
             <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1465,7 +1752,131 @@
           <xm:sqref>N5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{B31F4DC5-7A8C-804B-89A6-941728D02FBD}">
+          <x14:cfRule type="expression" priority="24" id="{EF4FC66B-04B7-8842-94D2-380B3463E6E7}">
+            <xm:f>$E6=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N6 N21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{079000E1-82CC-4547-A3B3-2FC477BD9AD9}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F7)))</xm:f>
+            <xm:f>Master!$C$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{C1FEE6D6-BA9C-467E-9139-40A64EBB3BB2}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F7)))</xm:f>
+            <xm:f>Master!$C$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{6CBC3277-9D41-4705-8AB5-58629FA1061E}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F7)))</xm:f>
+            <xm:f>Master!$C$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="10" id="{EB783649-1D40-4BE0-92EB-B8CA4BFE7B63}">
+            <xm:f>$E7=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B7:K7 M7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="9" id="{03632C2A-CCC1-45B6-939B-140F7A643C30}">
+            <xm:f>$E7=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="8" id="{3FC1C540-5099-4506-9A17-63068A6FB032}">
+            <xm:f>$E7=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{048BEF91-A2AA-4983-88CD-33E73F02E32B}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F8)))</xm:f>
+            <xm:f>Master!$C$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B0F0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{E9B99BF9-3AB4-44DC-BC24-D150D3D85A9C}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F8)))</xm:f>
+            <xm:f>Master!$C$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{220CC212-FADD-4B1F-AD96-A19DBB49A6E7}">
+            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F8)))</xm:f>
+            <xm:f>Master!$C$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F8:F20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{1FEF672A-E544-4EB2-99EB-C103B14065DA}">
             <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1475,47 +1886,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E8</xm:sqref>
+          <xm:sqref>B8:K20 M8:M20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{5EDD22EA-270F-064D-9ACE-ACAC46F7D7D3}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F9)))</xm:f>
-            <xm:f>Master!$C$4</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B0F0"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{30D1F81A-DEC7-E444-96B7-C79FBC52E21B}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F9)))</xm:f>
-            <xm:f>Master!$C$3</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{B3F98871-AEB5-664B-8DE2-9210588F29DB}">
-            <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F9)))</xm:f>
-            <xm:f>Master!$C$2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{CCCC3B6D-E61F-CE41-9FC8-5896F04EB6CF}">
-            <xm:f>$E9=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="2" id="{30AEF840-97EF-46B0-B6BF-95B98A5A237B}">
+            <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1524,11 +1899,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>L8:L20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{B73FD618-63AE-DF4C-A7CA-7FD2F8AE6608}">
-            <xm:f>$E9=Master!$A$4</xm:f>
+          <x14:cfRule type="expression" priority="1" id="{B362C712-D1C8-4407-90E9-3EDE3D0F4D42}">
+            <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1537,33 +1912,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{5669D208-A0FB-3B42-B58D-7CCD73284DA4}">
-            <xm:f>$E9=Master!$A$4</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.14996795556505021"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{EF4FC66B-04B7-8842-94D2-380B3463E6E7}">
-            <xm:f>$E6=Master!$A$4</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.14996795556505021"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>N6:N21</xm:sqref>
+          <xm:sqref>N8:N20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1573,19 +1922,19 @@
           <x14:formula1>
             <xm:f>Master!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F9</xm:sqref>
+          <xm:sqref>F3:F10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02CAAD53-6806-422A-96A9-575F68CB0F26}">
           <x14:formula1>
             <xm:f>Master!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E6 E8:E9</xm:sqref>
+          <xm:sqref>E3:E10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C020BD32-2477-4C5E-A522-B6AF819E784D}">
           <x14:formula1>
             <xm:f>Master!$D$2:$D$21</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C9</xm:sqref>
+          <xm:sqref>C5:C10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DC8D81E-F3FE-4360-B3D1-FE031C309CEE}">
           <x14:formula1>
@@ -1607,64 +1956,64 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="13" t="s">
         <v>17</v>
       </c>
@@ -1677,13 +2026,13 @@
       <c r="I2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -1731,7 +2080,7 @@
       <c r="L5" s="10"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -1740,7 +2089,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="16" thickBot="1">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -1764,12 +2113,12 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L6">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula xml:space="preserve"> AND(L7&lt;100, K7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1869,7 +2218,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1889,9 +2238,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
change schedule + add more bug
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D23368-1DDD-444B-B5D9-69B1342BCFDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54526926-6A76-4388-9ABB-D85E8C739B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1117,7 +1124,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J12"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1126,9 +1133,10 @@
     <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" customWidth="1"/>
     <col min="13" max="13" width="10.140625" customWidth="1"/>
@@ -1492,7 +1500,7 @@
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
@@ -1651,17 +1659,17 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" dxfId="44" priority="37">
+    <cfRule type="expression" dxfId="45" priority="37">
       <formula xml:space="preserve"> AND(M3&lt;100, L3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula xml:space="preserve"> AND(M7&lt;100, L7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:M20">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula xml:space="preserve"> AND(M8&lt;100, L8 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2113,12 +2121,12 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L6">
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula xml:space="preserve"> AND(L7&lt;100, K7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update shedule of Vy
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Desktop\Talent\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BAA179-C2C8-4C65-9F8C-84142B41E98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F4903-E15E-40D4-AB2F-E10524ADC3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>T6_Login_PT</t>
   </si>
   <si>
-    <t>T6_User Test (Mobile)</t>
-  </si>
-  <si>
     <t>LD_Home_Cd</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Mobile, Web, Tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T6_User Test </t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -461,12 +461,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -502,11 +517,8 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,12 +529,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -997,528 +1055,519 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="20.149999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" customWidth="1"/>
-    <col min="12" max="12" width="19.453125" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" customWidth="1"/>
-    <col min="14" max="14" width="23.453125" customWidth="1"/>
-    <col min="15" max="19" width="35.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="19" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="B1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>21</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.5">
-      <c r="B2" s="18"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="5" t="s">
+    <row r="2" spans="1:15" ht="15">
+      <c r="B2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="5" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="14.5">
-      <c r="A3">
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="20">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="20">
         <v>0.5</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="20">
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="20">
         <f t="shared" ref="J3:J4" si="0">SUM(G3:I3)</f>
         <v>0.5</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="24">
         <v>44111</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="24">
         <v>44111</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.5">
-      <c r="A4">
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+    </row>
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="20">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="20">
         <v>0.5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="20">
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="20">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="24">
         <v>44112</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="24">
         <v>44112</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="25">
         <v>100</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="26">
         <v>44112</v>
       </c>
-      <c r="O4" s="6"/>
+      <c r="O4" s="27"/>
     </row>
     <row r="5" spans="1:15" ht="81" customHeight="1">
-      <c r="A5">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="20">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="20">
         <v>1.5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="20">
         <v>0</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="20">
         <f>SUM(G5:I5)</f>
         <v>1.5</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="24">
         <v>44113</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="24">
         <v>44117</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="25">
         <v>100</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="28">
         <v>44118</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="A6">
+    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="20">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="20">
         <v>1.5</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="20">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="20">
         <f t="shared" ref="J6" si="1">SUM(G6:I6)</f>
         <v>1.5</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="24">
         <v>44118</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="24">
         <v>44118</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="25">
         <v>100</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="A7">
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="20">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="20">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="20">
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="20">
         <f t="shared" ref="J7" si="2">SUM(G7:I7)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="24">
         <v>44113</v>
       </c>
-      <c r="L7" s="9">
-        <v>44116</v>
-      </c>
-      <c r="M7" s="10">
-        <v>100</v>
-      </c>
-      <c r="N7" s="14"/>
-    </row>
-    <row r="8" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="A8">
+      <c r="L7" s="24">
+        <v>44135</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24">
+        <v>44119</v>
+      </c>
+      <c r="L8" s="24">
+        <v>44120</v>
+      </c>
+      <c r="M8" s="25">
+        <v>75</v>
+      </c>
+      <c r="N8" s="28"/>
+      <c r="O8" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="20">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24">
+        <v>44120</v>
+      </c>
+      <c r="L9" s="24">
+        <v>44120</v>
+      </c>
+      <c r="M9" s="25">
+        <v>15</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="20">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J8">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20">
         <v>1</v>
       </c>
-      <c r="K8" s="9">
-        <v>44119</v>
-      </c>
-      <c r="L8" s="9">
-        <v>44120</v>
-      </c>
-      <c r="M8" s="10">
-        <v>75</v>
-      </c>
-      <c r="N8" s="14"/>
-      <c r="O8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="9">
-        <v>44120</v>
-      </c>
-      <c r="L9" s="9">
-        <v>44120</v>
-      </c>
-      <c r="M9" s="10">
-        <v>15</v>
-      </c>
-      <c r="N9" s="14"/>
-      <c r="O9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="20.149999999999999" customHeight="1">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="K10" s="24">
+        <v>44125</v>
+      </c>
+      <c r="L10" s="24">
+        <v>44125</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="9">
-        <v>44120</v>
-      </c>
-      <c r="L10" s="9">
-        <v>44120</v>
-      </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="14"/>
-      <c r="O10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="20.149999999999999" customHeight="1">
+    </row>
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L11" s="9"/>
       <c r="M11" s="10"/>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:15" ht="20.149999999999999" customHeight="1">
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L12" s="9"/>
       <c r="M12" s="10"/>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:15" ht="20.149999999999999" customHeight="1">
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D13" s="2"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L13" s="9"/>
       <c r="M13" s="10"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:15" ht="20.149999999999999" customHeight="1">
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L14" s="9"/>
       <c r="M14" s="10"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="20.149999999999999" customHeight="1">
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L15" s="9"/>
       <c r="M15" s="10"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:15" ht="20.149999999999999" customHeight="1">
+    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L16" s="9"/>
       <c r="M16" s="10"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="4:14" ht="20.149999999999999" customHeight="1">
+    <row r="17" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L17" s="9"/>
       <c r="M17" s="10"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="4:14" ht="20.149999999999999" customHeight="1">
+    <row r="18" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L18" s="9"/>
       <c r="M18" s="10"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="4:14" ht="20.149999999999999" customHeight="1">
+    <row r="19" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L19" s="9"/>
       <c r="M19" s="10"/>
       <c r="N19" s="14"/>
     </row>
-    <row r="20" spans="4:14" ht="20.149999999999999" customHeight="1">
+    <row r="20" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="9">
-        <v>44120</v>
-      </c>
+      <c r="L20" s="9"/>
       <c r="M20" s="10"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="4:14" ht="20.149999999999999" customHeight="1">
+    <row r="21" spans="4:14" ht="20.100000000000001" customHeight="1">
       <c r="N21" s="14"/>
     </row>
   </sheetData>
@@ -1535,17 +1584,17 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M6">
-    <cfRule type="expression" dxfId="27" priority="37">
+    <cfRule type="expression" dxfId="30" priority="39">
       <formula xml:space="preserve"> AND(M3&lt;100, L3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="expression" dxfId="26" priority="11">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula xml:space="preserve"> AND(M7&lt;100, L7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:M20">
-    <cfRule type="expression" dxfId="25" priority="4">
+    <cfRule type="expression" dxfId="28" priority="6">
       <formula xml:space="preserve"> AND(M8&lt;100, L8 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1561,7 +1610,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="38" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
+          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{7B7EF211-77D1-4B43-B157-D287E441C828}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F1)))</xm:f>
             <xm:f>Master!$C$4</xm:f>
             <x14:dxf>
@@ -1572,7 +1621,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="39" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
+          <x14:cfRule type="containsText" priority="41" operator="containsText" id="{685FD9B1-64F0-4F8C-95F3-43B65EBBB91A}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F1)))</xm:f>
             <xm:f>Master!$C$3</xm:f>
             <x14:dxf>
@@ -1583,7 +1632,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="40" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
+          <x14:cfRule type="containsText" priority="42" operator="containsText" id="{9E26D091-31B5-4A3A-9D6D-22758EF9EF8C}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F1)))</xm:f>
             <xm:f>Master!$C$2</xm:f>
             <x14:dxf>
@@ -1597,7 +1646,7 @@
           <xm:sqref>F1:F6 F21:F1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="35" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
+          <x14:cfRule type="expression" priority="37" id="{DE2E40C7-EA13-48F8-8A97-1724515E75DA}">
             <xm:f>$E3=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1610,7 +1659,7 @@
           <xm:sqref>B5:K6 M5:M6 B3:O4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="33" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
+          <x14:cfRule type="expression" priority="35" id="{96EC7671-BCFD-4488-8EB5-371B09DF33C4}">
             <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1623,7 +1672,7 @@
           <xm:sqref>L5:L6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="32" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
+          <x14:cfRule type="expression" priority="34" id="{14A84CDC-2005-4B31-A017-37D0DF29D843}">
             <xm:f>$E5=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1636,7 +1685,7 @@
           <xm:sqref>N5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="24" id="{EF4FC66B-04B7-8842-94D2-380B3463E6E7}">
+          <x14:cfRule type="expression" priority="26" id="{EF4FC66B-04B7-8842-94D2-380B3463E6E7}">
             <xm:f>$E6=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1649,7 +1698,7 @@
           <xm:sqref>N6 N21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{079000E1-82CC-4547-A3B3-2FC477BD9AD9}">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{079000E1-82CC-4547-A3B3-2FC477BD9AD9}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F7)))</xm:f>
             <xm:f>Master!$C$4</xm:f>
             <x14:dxf>
@@ -1660,7 +1709,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{C1FEE6D6-BA9C-467E-9139-40A64EBB3BB2}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{C1FEE6D6-BA9C-467E-9139-40A64EBB3BB2}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F7)))</xm:f>
             <xm:f>Master!$C$3</xm:f>
             <x14:dxf>
@@ -1671,7 +1720,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{6CBC3277-9D41-4705-8AB5-58629FA1061E}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{6CBC3277-9D41-4705-8AB5-58629FA1061E}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F7)))</xm:f>
             <xm:f>Master!$C$2</xm:f>
             <x14:dxf>
@@ -1685,7 +1734,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="10" id="{EB783649-1D40-4BE0-92EB-B8CA4BFE7B63}">
+          <x14:cfRule type="expression" priority="12" id="{EB783649-1D40-4BE0-92EB-B8CA4BFE7B63}">
             <xm:f>$E7=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1698,7 +1747,7 @@
           <xm:sqref>B7:K7 M7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{03632C2A-CCC1-45B6-939B-140F7A643C30}">
+          <x14:cfRule type="expression" priority="11" id="{03632C2A-CCC1-45B6-939B-140F7A643C30}">
             <xm:f>$E7=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1711,7 +1760,7 @@
           <xm:sqref>L7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{3FC1C540-5099-4506-9A17-63068A6FB032}">
+          <x14:cfRule type="expression" priority="10" id="{3FC1C540-5099-4506-9A17-63068A6FB032}">
             <xm:f>$E7=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1724,7 +1773,7 @@
           <xm:sqref>N7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{048BEF91-A2AA-4983-88CD-33E73F02E32B}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{048BEF91-A2AA-4983-88CD-33E73F02E32B}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$4,F8)))</xm:f>
             <xm:f>Master!$C$4</xm:f>
             <x14:dxf>
@@ -1735,7 +1784,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{E9B99BF9-3AB4-44DC-BC24-D150D3D85A9C}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{E9B99BF9-3AB4-44DC-BC24-D150D3D85A9C}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$3,F8)))</xm:f>
             <xm:f>Master!$C$3</xm:f>
             <x14:dxf>
@@ -1746,7 +1795,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{220CC212-FADD-4B1F-AD96-A19DBB49A6E7}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{220CC212-FADD-4B1F-AD96-A19DBB49A6E7}">
             <xm:f>NOT(ISERROR(SEARCH(Master!$C$2,F8)))</xm:f>
             <xm:f>Master!$C$2</xm:f>
             <x14:dxf>
@@ -1760,7 +1809,7 @@
           <xm:sqref>F8:F20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{1FEF672A-E544-4EB2-99EB-C103B14065DA}">
+          <x14:cfRule type="expression" priority="5" id="{1FEF672A-E544-4EB2-99EB-C103B14065DA}">
             <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1773,7 +1822,7 @@
           <xm:sqref>B8:K20 M8:M20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{30AEF840-97EF-46B0-B6BF-95B98A5A237B}">
+          <x14:cfRule type="expression" priority="4" id="{30AEF840-97EF-46B0-B6BF-95B98A5A237B}">
             <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1783,10 +1832,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>L8:L20</xm:sqref>
+          <xm:sqref>L8:L10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{B362C712-D1C8-4407-90E9-3EDE3D0F4D42}">
+          <x14:cfRule type="expression" priority="3" id="{B362C712-D1C8-4407-90E9-3EDE3D0F4D42}">
             <xm:f>$E8=Master!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1797,6 +1846,19 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>N8:N20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{99B88758-3753-4E9B-8CF7-55E11445C430}">
+            <xm:f>$E11=Master!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.14996795556505021"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L11:L20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1840,64 +1902,64 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.453125" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="18.1796875" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="18"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="13" t="s">
         <v>17</v>
       </c>
@@ -1910,13 +1972,13 @@
       <c r="I2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -1964,7 +2026,7 @@
       <c r="L5" s="10"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
@@ -1973,7 +2035,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -1997,12 +2059,12 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L6">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula xml:space="preserve"> AND(L3&lt;100, K3 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula xml:space="preserve"> AND(L7&lt;100, K7 &lt; TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2102,7 +2164,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -2122,9 +2184,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>